<commit_message>
Features 1 qui fonctionne (youhou !)
Enregistrement des valeurs dans l'excel test
</commit_message>
<xml_diff>
--- a/train/testratio.xlsx
+++ b/train/testratio.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Bug Pixel Ratio</t>
+          <t>Bug Symmetry Index</t>
         </is>
       </c>
     </row>
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.007428041666666667</v>
+        <v>1.3034375</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.01578345833333333</v>
+        <v>5.419582</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.02534066666666667</v>
+        <v>4.64066</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0257145</v>
+        <v>4.201295</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.02665416666666667</v>
+        <v>6.307595</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.02822516666666667</v>
+        <v>4.068695</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.02492716666666667</v>
+        <v>7.524115</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.02371083333333333</v>
+        <v>1.332375</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0315595</v>
+        <v>9.435255</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.021639</v>
+        <v>11.03589</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.0153065</v>
+        <v>1.690735</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.03264966666666667</v>
+        <v>11.47466</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.01363091666666667</v>
+        <v>5.461257</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.021689</v>
+        <v>2.1264025</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.02168833333333333</v>
+        <v>6.80408</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.04435916666666666</v>
+        <v>10.018695</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.02879733333333333</v>
+        <v>7.33941</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.01853133333333333</v>
+        <v>3.90388</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.01457866666666667</v>
+        <v>7.43512</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.02898766666666667</v>
+        <v>4.34299</v>
       </c>
     </row>
     <row r="22">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.03543516666666666</v>
+        <v>17.951065</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.037257</v>
+        <v>17.0289</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.015522</v>
+        <v>5.4247</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.01804008333333334</v>
+        <v>5.023238166666666</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.02839925</v>
+        <v>13.8269075</v>
       </c>
     </row>
     <row r="27">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.018408125</v>
+        <v>6.31207875</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.02715133333333333</v>
+        <v>9.247405000000001</v>
       </c>
     </row>
     <row r="29">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.0302785</v>
+        <v>10.7657175</v>
       </c>
     </row>
     <row r="30">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.032656375</v>
+        <v>16.65475125</v>
       </c>
     </row>
     <row r="31">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.03888220833333333</v>
+        <v>6.75777625</v>
       </c>
     </row>
     <row r="32">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.04084775</v>
+        <v>7.22092</v>
       </c>
     </row>
     <row r="33">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.03217033333333334</v>
+        <v>16.40687</v>
       </c>
     </row>
     <row r="34">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.04239645833333333</v>
+        <v>21.62219375</v>
       </c>
     </row>
     <row r="35">
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.030271125</v>
+        <v>13.00927125</v>
       </c>
     </row>
     <row r="36">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.01632</v>
+        <v>6.544912416666667</v>
       </c>
     </row>
     <row r="37">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.02017875</v>
+        <v>5.1660025</v>
       </c>
     </row>
     <row r="38">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.03304125</v>
+        <v>5.275695</v>
       </c>
     </row>
     <row r="39">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.030832875</v>
+        <v>15.72476625</v>
       </c>
     </row>
     <row r="40">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.03890025</v>
+        <v>17.605965</v>
       </c>
     </row>
     <row r="41">
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.03878133333333333</v>
+        <v>10.846085</v>
       </c>
     </row>
     <row r="42">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.020028</v>
+        <v>7.63062</v>
       </c>
     </row>
     <row r="43">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.035679375</v>
+        <v>3.84801375</v>
       </c>
     </row>
     <row r="44">
@@ -872,7 +872,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.0216115</v>
+        <v>3.7068075</v>
       </c>
     </row>
     <row r="45">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.029323125</v>
+        <v>4.43056125</v>
       </c>
     </row>
     <row r="46">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.024273375</v>
+        <v>5.55064875</v>
       </c>
     </row>
     <row r="47">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.01099604166666667</v>
+        <v>3.193417</v>
       </c>
     </row>
     <row r="48">
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.021783875</v>
+        <v>11.09116125</v>
       </c>
     </row>
     <row r="49">
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.02043954166666667</v>
+        <v>6.66278875</v>
       </c>
     </row>
     <row r="50">
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.0185875</v>
+        <v>9.479625</v>
       </c>
     </row>
     <row r="51">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.008538125000000001</v>
+        <v>3.54775125</v>
       </c>
     </row>
     <row r="52">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.00873025</v>
+        <v>4.4524275</v>
       </c>
     </row>
     <row r="53">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.007945208333333334</v>
+        <v>4.05205625</v>
       </c>
     </row>
     <row r="54">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.02707825</v>
+        <v>3.3133425</v>
       </c>
     </row>
     <row r="55">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.02157225</v>
+        <v>5.1844475</v>
       </c>
     </row>
     <row r="56">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.028808875</v>
+        <v>12.70237875</v>
       </c>
     </row>
     <row r="57">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.01523766666666667</v>
+        <v>7.77121</v>
       </c>
     </row>
     <row r="58">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.01596066666666667</v>
+        <v>7.531411416666667</v>
       </c>
     </row>
     <row r="59">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.01668425</v>
+        <v>8.508967500000001</v>
       </c>
     </row>
     <row r="60">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.01417883333333333</v>
+        <v>1.70782</v>
       </c>
     </row>
     <row r="61">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.029318</v>
+        <v>5.835675</v>
       </c>
     </row>
     <row r="62">
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.033310875</v>
+        <v>15.21485125</v>
       </c>
     </row>
     <row r="63">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.007896625000000001</v>
+        <v>1.88476875</v>
       </c>
     </row>
     <row r="64">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.01543379166666667</v>
+        <v>7.18018375</v>
       </c>
     </row>
     <row r="65">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.03779220833333333</v>
+        <v>7.07002375</v>
       </c>
     </row>
     <row r="66">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.018113875</v>
+        <v>9.238076250000001</v>
       </c>
     </row>
     <row r="67">
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.02211375</v>
+        <v>11.2780125</v>
       </c>
     </row>
     <row r="68">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.01680670833333333</v>
+        <v>4.182193833333334</v>
       </c>
     </row>
     <row r="69">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.032661625</v>
+        <v>16.65742875</v>
       </c>
     </row>
     <row r="70">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.021076625</v>
+        <v>8.159001249999999</v>
       </c>
     </row>
     <row r="71">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.01761625</v>
+        <v>6.276825</v>
       </c>
     </row>
     <row r="72">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.026548125</v>
+        <v>7.85457375</v>
       </c>
     </row>
     <row r="73">
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.034155375</v>
+        <v>6.02329125</v>
       </c>
     </row>
     <row r="74">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.012401</v>
+        <v>2.27613</v>
       </c>
     </row>
     <row r="75">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.01354866666666667</v>
+        <v>3.8045575</v>
       </c>
     </row>
     <row r="76">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.01588145833333333</v>
+        <v>5.03661125</v>
       </c>
     </row>
     <row r="77">
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.01920825</v>
+        <v>2.7259925</v>
       </c>
     </row>
     <row r="78">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.024756</v>
+        <v>5.968275</v>
       </c>
     </row>
     <row r="79">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.01479166666666667</v>
+        <v>3.581018833333333</v>
       </c>
     </row>
     <row r="80">
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.01303245833333333</v>
+        <v>2.60004375</v>
       </c>
     </row>
     <row r="81">
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.02132279166666667</v>
+        <v>9.967886249999999</v>
       </c>
     </row>
     <row r="82">
@@ -1252,7 +1252,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.020887875</v>
+        <v>10.11255625</v>
       </c>
     </row>
     <row r="83">
@@ -1262,7 +1262,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.012898375</v>
+        <v>1.64336875</v>
       </c>
     </row>
     <row r="84">
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.022444125</v>
+        <v>10.87636625</v>
       </c>
     </row>
     <row r="85">
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.030173125</v>
+        <v>7.10436375</v>
       </c>
     </row>
     <row r="86">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.02764391666666667</v>
+        <v>9.636407500000001</v>
       </c>
     </row>
     <row r="87">
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.02409025</v>
+        <v>11.87892</v>
       </c>
     </row>
     <row r="88">
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0.026822125</v>
+        <v>3.54473375</v>
       </c>
     </row>
     <row r="89">
@@ -1322,7 +1322,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.01685245833333333</v>
+        <v>3.86577875</v>
       </c>
     </row>
     <row r="90">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.013739375</v>
+        <v>3.359672333333333</v>
       </c>
     </row>
     <row r="91">
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.015003875</v>
+        <v>5.31817375</v>
       </c>
     </row>
     <row r="92">
@@ -1352,7 +1352,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.012524125</v>
+        <v>4.81913875</v>
       </c>
     </row>
     <row r="93">
@@ -1362,7 +1362,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.014082125</v>
+        <v>4.37174125</v>
       </c>
     </row>
     <row r="94">
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0.02441508333333333</v>
+        <v>4.72566</v>
       </c>
     </row>
     <row r="95">
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>0.02372025</v>
+        <v>8.335397499999999</v>
       </c>
     </row>
     <row r="96">
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0.02372025</v>
+        <v>8.335397499999999</v>
       </c>
     </row>
     <row r="97">
@@ -1402,7 +1402,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>0.01897225</v>
+        <v>4.944365</v>
       </c>
     </row>
     <row r="98">
@@ -1412,7 +1412,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>0.0105845</v>
+        <v>1.9820725</v>
       </c>
     </row>
     <row r="99">
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.037367875</v>
+        <v>11.50821375</v>
       </c>
     </row>
     <row r="100">
@@ -1432,7 +1432,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.03958004166666667</v>
+        <v>13.56045375</v>
       </c>
     </row>
     <row r="101">
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>0.01237495833333333</v>
+        <v>2.228736666666667</v>
       </c>
     </row>
     <row r="102">
@@ -1452,7 +1452,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.023845125</v>
+        <v>8.37273375</v>
       </c>
     </row>
     <row r="103">
@@ -1462,7 +1462,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.011769375</v>
+        <v>6.00238125</v>
       </c>
     </row>
     <row r="104">
@@ -1472,7 +1472,7 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0.0324855</v>
+        <v>14.7107375</v>
       </c>
     </row>
     <row r="105">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.041817125</v>
+        <v>14.17066875</v>
       </c>
     </row>
     <row r="106">
@@ -1492,7 +1492,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0.022354625</v>
+        <v>5.55149875</v>
       </c>
     </row>
     <row r="107">
@@ -1502,7 +1502,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.024717625</v>
+        <v>4.67000625</v>
       </c>
     </row>
     <row r="108">
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.02660525</v>
+        <v>8.299569999999999</v>
       </c>
     </row>
     <row r="109">
@@ -1522,7 +1522,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0.023532875</v>
+        <v>7.16275875</v>
       </c>
     </row>
     <row r="110">
@@ -1532,7 +1532,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.02349525</v>
+        <v>9.221819999999999</v>
       </c>
     </row>
     <row r="111">
@@ -1542,7 +1542,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.03651925</v>
+        <v>10.1249875</v>
       </c>
     </row>
     <row r="112">
@@ -1552,7 +1552,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0.008553</v>
+        <v>1.792838166666667</v>
       </c>
     </row>
     <row r="113">
@@ -1562,7 +1562,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.019336625</v>
+        <v>6.244521083333333</v>
       </c>
     </row>
     <row r="114">
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>0.02837670833333333</v>
+        <v>4.76371875</v>
       </c>
     </row>
     <row r="115">
@@ -1582,7 +1582,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>0.020289625</v>
+        <v>10.26402625</v>
       </c>
     </row>
     <row r="116">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0.03662225</v>
+        <v>18.6773475</v>
       </c>
     </row>
     <row r="117">
@@ -1602,7 +1602,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>0.06901879166666666</v>
+        <v>17.19390625</v>
       </c>
     </row>
     <row r="118">
@@ -1612,7 +1612,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>0.03745425</v>
+        <v>6.3810775</v>
       </c>
     </row>
     <row r="119">
@@ -1622,7 +1622,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>0.034826875</v>
+        <v>8.788298749999999</v>
       </c>
     </row>
     <row r="120">
@@ -1632,7 +1632,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.02162304166666667</v>
+        <v>6.15759125</v>
       </c>
     </row>
     <row r="121">
@@ -1642,7 +1642,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>0.0633095</v>
+        <v>27.9985325</v>
       </c>
     </row>
     <row r="122">
@@ -1652,7 +1652,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>0.02710066666666667</v>
+        <v>6.2675175</v>
       </c>
     </row>
     <row r="123">
@@ -1662,7 +1662,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>0.010833</v>
+        <v>1.7433075</v>
       </c>
     </row>
     <row r="124">
@@ -1672,7 +1672,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>0.01604379166666667</v>
+        <v>3.951357333333333</v>
       </c>
     </row>
     <row r="125">
@@ -1682,7 +1682,7 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>0.012324125</v>
+        <v>3.86752125</v>
       </c>
     </row>
     <row r="126">
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>0.013546875</v>
+        <v>5.74712625</v>
       </c>
     </row>
     <row r="127">
@@ -1702,7 +1702,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>0.006400375</v>
+        <v>3.21140625</v>
       </c>
     </row>
     <row r="128">
@@ -1712,7 +1712,7 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>0.013624</v>
+        <v>3.002115</v>
       </c>
     </row>
     <row r="129">
@@ -1722,7 +1722,7 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>0.03511875</v>
+        <v>5.940395</v>
       </c>
     </row>
     <row r="130">
@@ -1732,7 +1732,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>0.016076375</v>
+        <v>7.47679125</v>
       </c>
     </row>
     <row r="131">
@@ -1742,7 +1742,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>0.0360285</v>
+        <v>11.511465</v>
       </c>
     </row>
     <row r="132">
@@ -1752,7 +1752,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0.02317775</v>
+        <v>9.391735000000001</v>
       </c>
     </row>
     <row r="133">
@@ -1762,7 +1762,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>0.019377375</v>
+        <v>4.28720875</v>
       </c>
     </row>
     <row r="134">
@@ -1772,7 +1772,7 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>0.04788425</v>
+        <v>10.56771</v>
       </c>
     </row>
     <row r="135">
@@ -1782,7 +1782,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>0.01381341666666667</v>
+        <v>5.4382495</v>
       </c>
     </row>
     <row r="136">
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>0.04341616666666667</v>
+        <v>7.534995</v>
       </c>
     </row>
     <row r="137">
@@ -1802,7 +1802,7 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>0.038485875</v>
+        <v>5.32765125</v>
       </c>
     </row>
     <row r="138">
@@ -1812,7 +1812,7 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>0.0401345</v>
+        <v>5.853865</v>
       </c>
     </row>
     <row r="139">
@@ -1822,7 +1822,7 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>0.007721125</v>
+        <v>3.93777375</v>
       </c>
     </row>
     <row r="140">
@@ -1832,7 +1832,7 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>0.022474</v>
+        <v>6.1030425</v>
       </c>
     </row>
     <row r="141">
@@ -1842,7 +1842,7 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>0.032730125</v>
+        <v>16.68352375</v>
       </c>
     </row>
     <row r="142">
@@ -1852,7 +1852,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>0.02533125</v>
+        <v>12.6541625</v>
       </c>
     </row>
     <row r="143">
@@ -1862,7 +1862,7 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>0.029271</v>
+        <v>9.4169375</v>
       </c>
     </row>
     <row r="144">
@@ -1872,7 +1872,7 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>0.0130305</v>
+        <v>5.4510075</v>
       </c>
     </row>
     <row r="145">
@@ -1882,7 +1882,7 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>0.026777</v>
+        <v>7.133115</v>
       </c>
     </row>
     <row r="146">
@@ -1892,7 +1892,7 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>0.01677391666666667</v>
+        <v>8.375045249999999</v>
       </c>
     </row>
     <row r="147">
@@ -1902,7 +1902,7 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>0.026699625</v>
+        <v>8.41493625</v>
       </c>
     </row>
     <row r="148">
@@ -1912,7 +1912,7 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>0.01730241666666667</v>
+        <v>6.3958675</v>
       </c>
     </row>
     <row r="149">
@@ -1922,7 +1922,7 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>0.008178208333333332</v>
+        <v>0.81869875</v>
       </c>
     </row>
     <row r="150">
@@ -1932,7 +1932,7 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>0.0129755</v>
+        <v>6.617505</v>
       </c>
     </row>
     <row r="151">
@@ -1942,7 +1942,7 @@
         </is>
       </c>
       <c r="B151" t="n">
-        <v>0.03939170833333333</v>
+        <v>20.03613625</v>
       </c>
     </row>
     <row r="152">
@@ -1952,7 +1952,7 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>0.007349916666666667</v>
+        <v>2.744395</v>
       </c>
     </row>
     <row r="153">
@@ -1962,7 +1962,7 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>0.1181235</v>
+        <v>32.3537625</v>
       </c>
     </row>
     <row r="154">
@@ -1972,7 +1972,7 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>0.0686645</v>
+        <v>8.0469075</v>
       </c>
     </row>
     <row r="155">
@@ -1982,7 +1982,7 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>0.07400491666666667</v>
+        <v>32.375905</v>
       </c>
     </row>
     <row r="156">
@@ -1992,7 +1992,7 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>0.022765875</v>
+        <v>5.25506125</v>
       </c>
     </row>
     <row r="157">
@@ -2002,7 +2002,7 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>0.02250479166666667</v>
+        <v>7.489567666666667</v>
       </c>
     </row>
     <row r="158">
@@ -2012,7 +2012,7 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>0.02347975</v>
+        <v>5.46839</v>
       </c>
     </row>
     <row r="159">
@@ -2022,7 +2022,7 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>0.02035591666666667</v>
+        <v>5.4443775</v>
       </c>
     </row>
     <row r="160">
@@ -2032,7 +2032,7 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>0.02675120833333333</v>
+        <v>9.55682625</v>
       </c>
     </row>
     <row r="161">
@@ -2042,7 +2042,7 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>0.024148125</v>
+        <v>8.738956249999999</v>
       </c>
     </row>
     <row r="162">
@@ -2052,7 +2052,7 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>0.006230625</v>
+        <v>1.11704875</v>
       </c>
     </row>
     <row r="163">
@@ -2062,7 +2062,7 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>0.007295375</v>
+        <v>3.72064125</v>
       </c>
     </row>
     <row r="164">
@@ -2072,7 +2072,7 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>0.00625025</v>
+        <v>2.4058825</v>
       </c>
     </row>
     <row r="165">
@@ -2082,7 +2082,7 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>0.020050375</v>
+        <v>4.58925625</v>
       </c>
     </row>
     <row r="166">
@@ -2092,7 +2092,7 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>0.0070325</v>
+        <v>2.61256</v>
       </c>
     </row>
     <row r="167">
@@ -2102,7 +2102,7 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>0.01195925</v>
+        <v>5.995815</v>
       </c>
     </row>
     <row r="168">
@@ -2112,7 +2112,7 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>0.01148145833333333</v>
+        <v>1.77454475</v>
       </c>
     </row>
     <row r="169">
@@ -2122,7 +2122,7 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>0.02336666666666667</v>
+        <v>11.917</v>
       </c>
     </row>
     <row r="170">
@@ -2132,7 +2132,7 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>0.01638866666666667</v>
+        <v>3.417809916666667</v>
       </c>
     </row>
     <row r="171">
@@ -2142,7 +2142,7 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>0.003765041666666667</v>
+        <v>1.844860833333333</v>
       </c>
     </row>
     <row r="172">
@@ -2152,7 +2152,7 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>0.0075635</v>
+        <v>2.547102166666666</v>
       </c>
     </row>
     <row r="173">
@@ -2162,7 +2162,7 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>0.01492520833333333</v>
+        <v>4.713078833333333</v>
       </c>
     </row>
     <row r="174">
@@ -2172,7 +2172,7 @@
         </is>
       </c>
       <c r="B174" t="n">
-        <v>0.022093125</v>
+        <v>8.820087416666667</v>
       </c>
     </row>
     <row r="175">
@@ -2182,7 +2182,7 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>0.01785545833333333</v>
+        <v>8.826546</v>
       </c>
     </row>
     <row r="176">
@@ -2192,7 +2192,7 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>0.011362125</v>
+        <v>1.95871875</v>
       </c>
     </row>
     <row r="177">
@@ -2202,7 +2202,7 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>0.009864166666666667</v>
+        <v>2.249015</v>
       </c>
     </row>
     <row r="178">
@@ -2212,7 +2212,7 @@
         </is>
       </c>
       <c r="B178" t="n">
-        <v>0.008155916666666667</v>
+        <v>4.1595175</v>
       </c>
     </row>
     <row r="179">
@@ -2222,7 +2222,7 @@
         </is>
       </c>
       <c r="B179" t="n">
-        <v>0.0080445</v>
+        <v>2.3511</v>
       </c>
     </row>
     <row r="180">
@@ -2232,7 +2232,7 @@
         </is>
       </c>
       <c r="B180" t="n">
-        <v>0.00541725</v>
+        <v>2.7627975</v>
       </c>
     </row>
     <row r="181">
@@ -2242,7 +2242,7 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>0.009457333333333333</v>
+        <v>4.131425</v>
       </c>
     </row>
     <row r="182">
@@ -2252,7 +2252,7 @@
         </is>
       </c>
       <c r="B182" t="n">
-        <v>0.0104475</v>
+        <v>5.28513</v>
       </c>
     </row>
     <row r="183">
@@ -2262,7 +2262,7 @@
         </is>
       </c>
       <c r="B183" t="n">
-        <v>0.01157</v>
+        <v>5.9007</v>
       </c>
     </row>
     <row r="184">
@@ -2272,7 +2272,7 @@
         </is>
       </c>
       <c r="B184" t="n">
-        <v>0.01658483333333333</v>
+        <v>5.253085</v>
       </c>
     </row>
     <row r="185">
@@ -2282,7 +2282,7 @@
         </is>
       </c>
       <c r="B185" t="n">
-        <v>0.013187375</v>
+        <v>6.532336833333333</v>
       </c>
     </row>
     <row r="186">
@@ -2292,7 +2292,7 @@
         </is>
       </c>
       <c r="B186" t="n">
-        <v>0.01470125</v>
+        <v>4.515285</v>
       </c>
     </row>
     <row r="187">
@@ -2302,7 +2302,7 @@
         </is>
       </c>
       <c r="B187" t="n">
-        <v>0.0093895</v>
+        <v>3.354525</v>
       </c>
     </row>
     <row r="188">
@@ -2312,7 +2312,7 @@
         </is>
       </c>
       <c r="B188" t="n">
-        <v>0.013253875</v>
+        <v>6.48624375</v>
       </c>
     </row>
     <row r="189">
@@ -2322,7 +2322,7 @@
         </is>
       </c>
       <c r="B189" t="n">
-        <v>0.01939133333333333</v>
+        <v>7.81983</v>
       </c>
     </row>
     <row r="190">
@@ -2332,7 +2332,7 @@
         </is>
       </c>
       <c r="B190" t="n">
-        <v>0.01255433333333333</v>
+        <v>4.87084</v>
       </c>
     </row>
     <row r="191">
@@ -2342,7 +2342,7 @@
         </is>
       </c>
       <c r="B191" t="n">
-        <v>0.01361541666666667</v>
+        <v>2.9300775</v>
       </c>
     </row>
     <row r="192">
@@ -2352,7 +2352,7 @@
         </is>
       </c>
       <c r="B192" t="n">
-        <v>0.02093445833333333</v>
+        <v>6.96925625</v>
       </c>
     </row>
     <row r="193">
@@ -2362,7 +2362,7 @@
         </is>
       </c>
       <c r="B193" t="n">
-        <v>0.012116</v>
+        <v>6.17916</v>
       </c>
     </row>
     <row r="194">
@@ -2372,7 +2372,7 @@
         </is>
       </c>
       <c r="B194" t="n">
-        <v>0.009546374999999999</v>
+        <v>3.06898875</v>
       </c>
     </row>
     <row r="195">
@@ -2382,7 +2382,7 @@
         </is>
       </c>
       <c r="B195" t="n">
-        <v>0.01780525</v>
+        <v>4.4129025</v>
       </c>
     </row>
     <row r="196">
@@ -2392,7 +2392,7 @@
         </is>
       </c>
       <c r="B196" t="n">
-        <v>0.009164624999999999</v>
+        <v>2.928977</v>
       </c>
     </row>
     <row r="197">
@@ -2402,7 +2402,7 @@
         </is>
       </c>
       <c r="B197" t="n">
-        <v>0.01984966666666667</v>
+        <v>6.72469</v>
       </c>
     </row>
     <row r="198">
@@ -2412,7 +2412,7 @@
         </is>
       </c>
       <c r="B198" t="n">
-        <v>0.02193633333333333</v>
+        <v>5.69925</v>
       </c>
     </row>
     <row r="199">
@@ -2422,7 +2422,7 @@
         </is>
       </c>
       <c r="B199" t="n">
-        <v>0.020392</v>
+        <v>3.87464</v>
       </c>
     </row>
     <row r="200">
@@ -2432,7 +2432,7 @@
         </is>
       </c>
       <c r="B200" t="n">
-        <v>0.0164825</v>
+        <v>8.406075</v>
       </c>
     </row>
     <row r="201">
@@ -2442,7 +2442,7 @@
         </is>
       </c>
       <c r="B201" t="n">
-        <v>0.01179075</v>
+        <v>4.2967925</v>
       </c>
     </row>
     <row r="202">
@@ -2452,7 +2452,7 @@
         </is>
       </c>
       <c r="B202" t="n">
-        <v>0.01345133333333333</v>
+        <v>2.9705375</v>
       </c>
     </row>
     <row r="203">
@@ -2462,7 +2462,7 @@
         </is>
       </c>
       <c r="B203" t="n">
-        <v>0.008527833333333333</v>
+        <v>1.553035</v>
       </c>
     </row>
     <row r="204">
@@ -2472,7 +2472,7 @@
         </is>
       </c>
       <c r="B204" t="n">
-        <v>0.007866333333333333</v>
+        <v>2.74567</v>
       </c>
     </row>
     <row r="205">
@@ -2482,7 +2482,7 @@
         </is>
       </c>
       <c r="B205" t="n">
-        <v>0.01040366666666667</v>
+        <v>3.71144</v>
       </c>
     </row>
     <row r="206">
@@ -2492,7 +2492,7 @@
         </is>
       </c>
       <c r="B206" t="n">
-        <v>0.0114715</v>
+        <v>5.850465</v>
       </c>
     </row>
     <row r="207">
@@ -2502,7 +2502,7 @@
         </is>
       </c>
       <c r="B207" t="n">
-        <v>0.005916833333333333</v>
+        <v>2.928670416666667</v>
       </c>
     </row>
     <row r="208">
@@ -2512,7 +2512,7 @@
         </is>
       </c>
       <c r="B208" t="n">
-        <v>0.007962833333333334</v>
+        <v>3.12069</v>
       </c>
     </row>
     <row r="209">
@@ -2522,7 +2522,7 @@
         </is>
       </c>
       <c r="B209" t="n">
-        <v>0.01699683333333333</v>
+        <v>8.668385000000001</v>
       </c>
     </row>
     <row r="210">
@@ -2532,7 +2532,7 @@
         </is>
       </c>
       <c r="B210" t="n">
-        <v>0.0200545</v>
+        <v>10.227795</v>
       </c>
     </row>
     <row r="211">
@@ -2542,7 +2542,7 @@
         </is>
       </c>
       <c r="B211" t="n">
-        <v>0.01318483333333333</v>
+        <v>3.734645</v>
       </c>
     </row>
     <row r="212">
@@ -2552,7 +2552,7 @@
         </is>
       </c>
       <c r="B212" t="n">
-        <v>0.02632075</v>
+        <v>11.1357225</v>
       </c>
     </row>
     <row r="213">
@@ -2562,7 +2562,7 @@
         </is>
       </c>
       <c r="B213" t="n">
-        <v>0.02441283333333333</v>
+        <v>11.544615</v>
       </c>
     </row>
     <row r="214">
@@ -2572,7 +2572,7 @@
         </is>
       </c>
       <c r="B214" t="n">
-        <v>0.02465666666666667</v>
+        <v>9.0406</v>
       </c>
     </row>
     <row r="215">
@@ -2582,7 +2582,7 @@
         </is>
       </c>
       <c r="B215" t="n">
-        <v>0.01751033333333333</v>
+        <v>8.311299999999999</v>
       </c>
     </row>
     <row r="216">
@@ -2592,7 +2592,7 @@
         </is>
       </c>
       <c r="B216" t="n">
-        <v>0.0161465</v>
+        <v>8.234715</v>
       </c>
     </row>
     <row r="217">
@@ -2602,7 +2602,7 @@
         </is>
       </c>
       <c r="B217" t="n">
-        <v>0.017729</v>
+        <v>5.779405</v>
       </c>
     </row>
     <row r="218">
@@ -2612,7 +2612,7 @@
         </is>
       </c>
       <c r="B218" t="n">
-        <v>0.00565875</v>
+        <v>2.80438</v>
       </c>
     </row>
     <row r="219">
@@ -2622,7 +2622,7 @@
         </is>
       </c>
       <c r="B219" t="n">
-        <v>0.01526616666666667</v>
+        <v>2.0538125</v>
       </c>
     </row>
     <row r="220">
@@ -2632,7 +2632,7 @@
         </is>
       </c>
       <c r="B220" t="n">
-        <v>0.006874666666666667</v>
+        <v>3.50608</v>
       </c>
     </row>
     <row r="221">
@@ -2642,7 +2642,7 @@
         </is>
       </c>
       <c r="B221" t="n">
-        <v>0.0073725</v>
+        <v>3.759975</v>
       </c>
     </row>
     <row r="222">
@@ -2652,7 +2652,7 @@
         </is>
       </c>
       <c r="B222" t="n">
-        <v>0.01831016666666667</v>
+        <v>9.338184999999999</v>
       </c>
     </row>
     <row r="223">
@@ -2662,7 +2662,7 @@
         </is>
       </c>
       <c r="B223" t="n">
-        <v>0.01696533333333333</v>
+        <v>7.16312</v>
       </c>
     </row>
     <row r="224">
@@ -2672,7 +2672,7 @@
         </is>
       </c>
       <c r="B224" t="n">
-        <v>0.00476125</v>
+        <v>1.2730875</v>
       </c>
     </row>
     <row r="225">
@@ -2682,7 +2682,7 @@
         </is>
       </c>
       <c r="B225" t="n">
-        <v>0.013378</v>
+        <v>6.0554</v>
       </c>
     </row>
     <row r="226">
@@ -2692,7 +2692,7 @@
         </is>
       </c>
       <c r="B226" t="n">
-        <v>0.007123375</v>
+        <v>2.39821125</v>
       </c>
     </row>
     <row r="227">
@@ -2702,7 +2702,7 @@
         </is>
       </c>
       <c r="B227" t="n">
-        <v>0.01938683333333333</v>
+        <v>5.239655</v>
       </c>
     </row>
     <row r="228">
@@ -2712,7 +2712,7 @@
         </is>
       </c>
       <c r="B228" t="n">
-        <v>0.01279033333333333</v>
+        <v>6.52307</v>
       </c>
     </row>
     <row r="229">
@@ -2722,7 +2722,7 @@
         </is>
       </c>
       <c r="B229" t="n">
-        <v>0.007454083333333333</v>
+        <v>3.707533666666667</v>
       </c>
     </row>
     <row r="230">
@@ -2732,7 +2732,7 @@
         </is>
       </c>
       <c r="B230" t="n">
-        <v>0.012707</v>
+        <v>1.950325</v>
       </c>
     </row>
     <row r="231">
@@ -2742,7 +2742,7 @@
         </is>
       </c>
       <c r="B231" t="n">
-        <v>0.01563616666666667</v>
+        <v>4.116975</v>
       </c>
     </row>
     <row r="232">
@@ -2752,7 +2752,7 @@
         </is>
       </c>
       <c r="B232" t="n">
-        <v>0.04024433333333333</v>
+        <v>16.35978</v>
       </c>
     </row>
     <row r="233">
@@ -2762,7 +2762,7 @@
         </is>
       </c>
       <c r="B233" t="n">
-        <v>0.1874578333333333</v>
+        <v>20.1978275</v>
       </c>
     </row>
     <row r="234">
@@ -2772,7 +2772,7 @@
         </is>
       </c>
       <c r="B234" t="n">
-        <v>0.015821865720477</v>
+        <v>3.09753957074837</v>
       </c>
     </row>
     <row r="235">
@@ -2782,7 +2782,7 @@
         </is>
       </c>
       <c r="B235" t="n">
-        <v>0.05283633333333333</v>
+        <v>11.48775</v>
       </c>
     </row>
     <row r="236">
@@ -2792,7 +2792,7 @@
         </is>
       </c>
       <c r="B236" t="n">
-        <v>0.0253965</v>
+        <v>5.801845</v>
       </c>
     </row>
     <row r="237">
@@ -2802,7 +2802,7 @@
         </is>
       </c>
       <c r="B237" t="n">
-        <v>0.02543833333333333</v>
+        <v>2.6369125</v>
       </c>
     </row>
     <row r="238">
@@ -2812,7 +2812,7 @@
         </is>
       </c>
       <c r="B238" t="n">
-        <v>0.0432945</v>
+        <v>6.894775</v>
       </c>
     </row>
     <row r="239">
@@ -2822,7 +2822,7 @@
         </is>
       </c>
       <c r="B239" t="n">
-        <v>0.01983816666666667</v>
+        <v>7.221855</v>
       </c>
     </row>
     <row r="240">
@@ -2832,7 +2832,7 @@
         </is>
       </c>
       <c r="B240" t="n">
-        <v>0.007199416666666666</v>
+        <v>2.693312083333333</v>
       </c>
     </row>
     <row r="241">
@@ -2842,7 +2842,7 @@
         </is>
       </c>
       <c r="B241" t="n">
-        <v>0.0197255</v>
+        <v>3.666985</v>
       </c>
     </row>
     <row r="242">
@@ -2852,7 +2852,7 @@
         </is>
       </c>
       <c r="B242" t="n">
-        <v>0.03945316666666666</v>
+        <v>20.121115</v>
       </c>
     </row>
     <row r="243">
@@ -2862,7 +2862,7 @@
         </is>
       </c>
       <c r="B243" t="n">
-        <v>0.03404291666666667</v>
+        <v>17.3618875</v>
       </c>
     </row>
     <row r="244">
@@ -2872,7 +2872,7 @@
         </is>
       </c>
       <c r="B244" t="n">
-        <v>0.03879566666666667</v>
+        <v>7.47235</v>
       </c>
     </row>
     <row r="245">
@@ -2882,7 +2882,7 @@
         </is>
       </c>
       <c r="B245" t="n">
-        <v>0.0403435</v>
+        <v>15.668985</v>
       </c>
     </row>
     <row r="246">
@@ -2892,7 +2892,7 @@
         </is>
       </c>
       <c r="B246" t="n">
-        <v>0.02890683333333333</v>
+        <v>14.742485</v>
       </c>
     </row>
     <row r="247">
@@ -2902,7 +2902,7 @@
         </is>
       </c>
       <c r="B247" t="n">
-        <v>0.0365135</v>
+        <v>6.933195</v>
       </c>
     </row>
     <row r="248">
@@ -2912,7 +2912,7 @@
         </is>
       </c>
       <c r="B248" t="n">
-        <v>0.038646</v>
+        <v>3.48211</v>
       </c>
     </row>
     <row r="249">
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="B249" t="n">
-        <v>0.02642116666666667</v>
+        <v>10.787265</v>
       </c>
     </row>
     <row r="250">
@@ -2932,7 +2932,7 @@
         </is>
       </c>
       <c r="B250" t="n">
-        <v>0.0363615</v>
+        <v>15.373015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>